<commit_message>
Auto commit: 2025-04-15 21:24:21
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="MinVarPortfolio" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -59,6 +60,12 @@
   </si>
   <si>
     <t>Expected Shortfall 99%</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Asset</t>
   </si>
 </sst>
 </file>
@@ -612,4 +619,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit: 2025-04-15 21:43:49
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="MinVarPortfolio" sheetId="2" r:id="rId2"/>
+    <sheet name="MVP_Weights" sheetId="2" r:id="rId2"/>
+    <sheet name="MVP_Stats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -66,6 +67,15 @@
   </si>
   <si>
     <t>Asset</t>
+  </si>
+  <si>
+    <t>Portfolio Mean Return</t>
+  </si>
+  <si>
+    <t>Portfolio Standard Deviation</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
   </si>
 </sst>
 </file>
@@ -672,4 +682,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>0.00108357142866864</v>
+      </c>
+      <c r="C2">
+        <v>0.01091700535987142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit: 2025-04-15 22:13:15
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="MVP_Weights" sheetId="2" r:id="rId2"/>
-    <sheet name="MVP_Stats" sheetId="3" r:id="rId3"/>
+    <sheet name="Daily_Statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="Annual_Statistics" sheetId="2" r:id="rId2"/>
+    <sheet name="MVP_Weights" sheetId="3" r:id="rId3"/>
+    <sheet name="MVP_Stats" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -51,16 +52,16 @@
     <t>Kurtosis</t>
   </si>
   <si>
-    <t>Empirical VaR 95%</t>
-  </si>
-  <si>
-    <t>Expected Shortfall 95%</t>
-  </si>
-  <si>
-    <t>Empirical VaR 99%</t>
-  </si>
-  <si>
-    <t>Expected Shortfall 99%</t>
+    <t>VaR 95%</t>
+  </si>
+  <si>
+    <t>ES 95%</t>
+  </si>
+  <si>
+    <t>VaR 99%</t>
+  </si>
+  <si>
+    <t>ES 99%</t>
   </si>
   <si>
     <t>Weight</t>
@@ -461,16 +462,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>161.74</v>
+        <v>201.3</v>
       </c>
       <c r="C2">
-        <v>190.829</v>
+        <v>254.7</v>
       </c>
       <c r="D2">
-        <v>683.5</v>
+        <v>781.3</v>
       </c>
       <c r="E2">
-        <v>43.63</v>
+        <v>36.55</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -478,16 +479,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.001650284314457506</v>
+        <v>0.0004098013293508894</v>
       </c>
       <c r="C3">
-        <v>0.0004206590272864303</v>
+        <v>0.0006221043485396727</v>
       </c>
       <c r="D3">
-        <v>0.0004648066249659829</v>
+        <v>0.0002993732022570493</v>
       </c>
       <c r="E3">
-        <v>0.001798535747964639</v>
+        <v>-0.0001622489719508735</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -495,16 +496,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.01210495894101895</v>
+        <v>0.01382976152410843</v>
       </c>
       <c r="C4">
-        <v>0.008755609398051848</v>
+        <v>0.01190981747785037</v>
       </c>
       <c r="D4">
-        <v>0.009726073434777898</v>
+        <v>0.0127642524571061</v>
       </c>
       <c r="E4">
-        <v>0.02614468598933013</v>
+        <v>0.03150980377232784</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -512,16 +513,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.0001465300309637546</v>
+        <v>0.00019126230381371</v>
       </c>
       <c r="C5">
-        <v>7.666069593125384E-05</v>
+        <v>0.0001418437523557101</v>
       </c>
       <c r="D5">
-        <v>9.459650445869232E-05</v>
+        <v>0.0001629261407887392</v>
       </c>
       <c r="E5">
-        <v>0.0006835446054806749</v>
+        <v>0.0009928677337706061</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -529,16 +530,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.598275154235423</v>
+        <v>-0.1736236955280446</v>
       </c>
       <c r="C6">
-        <v>-0.104956455941808</v>
+        <v>-0.5310272909960784</v>
       </c>
       <c r="D6">
-        <v>-0.2001417301867452</v>
+        <v>-0.4348566222261216</v>
       </c>
       <c r="E6">
-        <v>0.3558744450200944</v>
+        <v>-0.7210069636931663</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -546,16 +547,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>2.130009561889286</v>
+        <v>1.355289324219858</v>
       </c>
       <c r="C7">
-        <v>1.688795061363862</v>
+        <v>5.926437800708015</v>
       </c>
       <c r="D7">
-        <v>0.7875659701474236</v>
+        <v>6.508584345364187</v>
       </c>
       <c r="E7">
-        <v>0.7185392133336488</v>
+        <v>6.518477693830253</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -563,16 +564,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-0.01889394101262612</v>
+        <v>-0.02391909987079396</v>
       </c>
       <c r="C8">
-        <v>-0.01368648895925294</v>
+        <v>-0.01736620301863545</v>
       </c>
       <c r="D8">
-        <v>-0.01474055034617178</v>
+        <v>-0.02043358709577255</v>
       </c>
       <c r="E8">
-        <v>-0.03970263886532165</v>
+        <v>-0.04868307573724512</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -580,16 +581,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-0.02199167942991705</v>
+        <v>-0.03128387024261594</v>
       </c>
       <c r="C9">
-        <v>-0.01860719318697671</v>
+        <v>-0.0281395131394166</v>
       </c>
       <c r="D9">
-        <v>-0.0212880502679782</v>
+        <v>-0.03068661573676915</v>
       </c>
       <c r="E9">
-        <v>-0.04921899791036756</v>
+        <v>-0.07146682517145642</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -597,16 +598,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-0.02453450233652399</v>
+        <v>-0.03644107693407325</v>
       </c>
       <c r="C10">
-        <v>-0.02075817221787528</v>
+        <v>-0.03352152295620385</v>
       </c>
       <c r="D10">
-        <v>-0.02439228953787581</v>
+        <v>-0.03661309409350758</v>
       </c>
       <c r="E10">
-        <v>-0.05326382679532255</v>
+        <v>-0.0752792562145345</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -614,16 +615,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.02655910682087396</v>
+        <v>-0.0442008868805281</v>
       </c>
       <c r="C11">
-        <v>-0.02810749015291655</v>
+        <v>-0.04985149434408001</v>
       </c>
       <c r="D11">
-        <v>-0.02971962558205153</v>
+        <v>-0.04873649174613838</v>
       </c>
       <c r="E11">
-        <v>-0.05807735089774701</v>
+        <v>-0.1242680872778185</v>
       </c>
     </row>
   </sheetData>
@@ -632,6 +633,206 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>201.3</v>
+      </c>
+      <c r="C2">
+        <v>254.7</v>
+      </c>
+      <c r="D2">
+        <v>781.3</v>
+      </c>
+      <c r="E2">
+        <v>36.55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0.1024503323377223</v>
+      </c>
+      <c r="C3">
+        <v>0.1555260871349182</v>
+      </c>
+      <c r="D3">
+        <v>0.07484330056426232</v>
+      </c>
+      <c r="E3">
+        <v>-0.04056224298771838</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.2186677295657215</v>
+      </c>
+      <c r="C4">
+        <v>0.1883107487344456</v>
+      </c>
+      <c r="D4">
+        <v>0.2018205519692798</v>
+      </c>
+      <c r="E4">
+        <v>0.4982137427276083</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.0478155759534275</v>
+      </c>
+      <c r="C5">
+        <v>0.03546093808892752</v>
+      </c>
+      <c r="D5">
+        <v>0.04073153519718479</v>
+      </c>
+      <c r="E5">
+        <v>0.2482169334426515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>-0.1736236955280446</v>
+      </c>
+      <c r="C6">
+        <v>-0.5310272909960784</v>
+      </c>
+      <c r="D6">
+        <v>-0.4348566222261216</v>
+      </c>
+      <c r="E6">
+        <v>-0.7210069636931663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1.355289324219858</v>
+      </c>
+      <c r="C7">
+        <v>5.926437800708015</v>
+      </c>
+      <c r="D7">
+        <v>6.508584345364187</v>
+      </c>
+      <c r="E7">
+        <v>6.518477693830253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>-0.3781941758637406</v>
+      </c>
+      <c r="C8">
+        <v>-0.2745837792388978</v>
+      </c>
+      <c r="D8">
+        <v>-0.3230833799503321</v>
+      </c>
+      <c r="E8">
+        <v>-0.7697470141608774</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>-0.4946414199591536</v>
+      </c>
+      <c r="C9">
+        <v>-0.4449247688439585</v>
+      </c>
+      <c r="D9">
+        <v>-0.4851979970527825</v>
+      </c>
+      <c r="E9">
+        <v>-1.129989723414279</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>-0.5761840175054853</v>
+      </c>
+      <c r="C10">
+        <v>-0.5300218158961246</v>
+      </c>
+      <c r="D10">
+        <v>-0.5789038476077093</v>
+      </c>
+      <c r="E10">
+        <v>-1.19026955100657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>-0.6988773857096181</v>
+      </c>
+      <c r="C11">
+        <v>-0.7882213344514727</v>
+      </c>
+      <c r="D11">
+        <v>-0.77059159541897</v>
+      </c>
+      <c r="E11">
+        <v>-1.964850981352499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -684,7 +885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -705,10 +906,10 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>0.00108357142866864</v>
+        <v>0.000222138666407758</v>
       </c>
       <c r="C2">
-        <v>0.01091700535987142</v>
+        <v>0.01108004749581097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit: 2025-04-22 12:16:30
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -9,15 +9,13 @@
   <sheets>
     <sheet name="Daily_Statistics" sheetId="1" r:id="rId1"/>
     <sheet name="Annual_Statistics" sheetId="2" r:id="rId2"/>
-    <sheet name="MVP_Weights" sheetId="3" r:id="rId3"/>
-    <sheet name="MVP_Stats" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -62,21 +60,6 @@
   </si>
   <si>
     <t>ES 99%</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>Portfolio Mean Return</t>
-  </si>
-  <si>
-    <t>Portfolio Standard Deviation</t>
-  </si>
-  <si>
-    <t>Portfolio</t>
   </si>
 </sst>
 </file>
@@ -830,89 +813,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>0.000222138666407758</v>
-      </c>
-      <c r="C2">
-        <v>0.01108004749581097</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit: 2025-04-22 12:38:22
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Daily_Statistics" sheetId="1" r:id="rId1"/>
     <sheet name="Annual_Statistics" sheetId="2" r:id="rId2"/>
+    <sheet name="10Day_Statistics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -29,6 +30,9 @@
     <t>WIG20</t>
   </si>
   <si>
+    <t>APPLE</t>
+  </si>
+  <si>
     <t>Statistic</t>
   </si>
   <si>
@@ -60,6 +64,16 @@
   </si>
   <si>
     <t>ES 99%</t>
+  </si>
+  <si>
+    <t>Ticker
+AAPL    191.380951
+Name: 249, dtype: float64</t>
+  </si>
+  <si>
+    <t>Ticker
+AAPL    1913.809509
+Name: 249, dtype: float64</t>
   </si>
 </sst>
 </file>
@@ -417,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -439,175 +453,208 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>201.3</v>
+        <v>161.74</v>
       </c>
       <c r="C2">
-        <v>254.7</v>
+        <v>190.829</v>
       </c>
       <c r="D2">
-        <v>781.3</v>
+        <v>683.5</v>
       </c>
       <c r="E2">
-        <v>36.55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>43.63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.0004098013293508894</v>
+        <v>0.001650284314457506</v>
       </c>
       <c r="C3">
-        <v>0.0006221043485396727</v>
+        <v>0.0004206590272864303</v>
       </c>
       <c r="D3">
-        <v>0.0002993732022570493</v>
+        <v>0.0004648066249659829</v>
       </c>
       <c r="E3">
-        <v>-0.0001622489719508735</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0.001798535747964639</v>
+      </c>
+      <c r="F3">
+        <v>0.00175482855833993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.01382976152410843</v>
+        <v>0.01210495894101895</v>
       </c>
       <c r="C4">
-        <v>0.01190981747785037</v>
+        <v>0.008755609398051848</v>
       </c>
       <c r="D4">
-        <v>0.0127642524571061</v>
+        <v>0.009726073434777898</v>
       </c>
       <c r="E4">
-        <v>0.03150980377232784</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.02614468598933013</v>
+      </c>
+      <c r="F4">
+        <v>0.01254982478532658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.00019126230381371</v>
+        <v>0.0001465300309637546</v>
       </c>
       <c r="C5">
-        <v>0.0001418437523557101</v>
+        <v>7.666069593125384E-05</v>
       </c>
       <c r="D5">
-        <v>0.0001629261407887392</v>
+        <v>9.459650445869232E-05</v>
       </c>
       <c r="E5">
-        <v>0.0009928677337706061</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.0006835446054806749</v>
+      </c>
+      <c r="F5">
+        <v>0.0001574981021423972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>-0.1736236955280446</v>
+        <v>0.598275154235423</v>
       </c>
       <c r="C6">
-        <v>-0.5310272909960784</v>
+        <v>-0.104956455941808</v>
       </c>
       <c r="D6">
-        <v>-0.4348566222261216</v>
+        <v>-0.2001417301867452</v>
       </c>
       <c r="E6">
-        <v>-0.7210069636931663</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.3558744450200944</v>
+      </c>
+      <c r="F6">
+        <v>-0.05249116119637225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>1.355289324219858</v>
+        <v>2.130009561889286</v>
       </c>
       <c r="C7">
-        <v>5.926437800708015</v>
+        <v>1.688795061363862</v>
       </c>
       <c r="D7">
-        <v>6.508584345364187</v>
+        <v>0.7875659701474236</v>
       </c>
       <c r="E7">
-        <v>6.518477693830253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.7185392133336488</v>
+      </c>
+      <c r="F7">
+        <v>1.470637836340662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>-0.02391909987079396</v>
+        <v>-0.01889394101262612</v>
       </c>
       <c r="C8">
-        <v>-0.01736620301863545</v>
+        <v>-0.01368648895925294</v>
       </c>
       <c r="D8">
-        <v>-0.02043358709577255</v>
+        <v>-0.01474055034617178</v>
       </c>
       <c r="E8">
-        <v>-0.04868307573724512</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>-0.03970263886532165</v>
+      </c>
+      <c r="F8">
+        <v>-0.01732564416448271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>-0.03128387024261594</v>
+        <v>-0.02199167942991705</v>
       </c>
       <c r="C9">
-        <v>-0.0281395131394166</v>
+        <v>-0.01860719318697671</v>
       </c>
       <c r="D9">
-        <v>-0.03068661573676915</v>
+        <v>-0.0212880502679782</v>
       </c>
       <c r="E9">
-        <v>-0.07146682517145642</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>-0.04921899791036756</v>
+      </c>
+      <c r="F9">
+        <v>-0.02534234683392821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>-0.03644107693407325</v>
+        <v>-0.02453450233652399</v>
       </c>
       <c r="C10">
-        <v>-0.03352152295620385</v>
+        <v>-0.02075817221787528</v>
       </c>
       <c r="D10">
-        <v>-0.03661309409350758</v>
+        <v>-0.02439228953787581</v>
       </c>
       <c r="E10">
-        <v>-0.0752792562145345</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>-0.05326382679532255</v>
+      </c>
+      <c r="F10">
+        <v>-0.02841681210596071</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>-0.0442008868805281</v>
+        <v>-0.02655910682087396</v>
       </c>
       <c r="C11">
-        <v>-0.04985149434408001</v>
+        <v>-0.02810749015291655</v>
       </c>
       <c r="D11">
-        <v>-0.04873649174613838</v>
+        <v>-0.02971962558205153</v>
       </c>
       <c r="E11">
-        <v>-0.1242680872778185</v>
+        <v>-0.05807735089774701</v>
+      </c>
+      <c r="F11">
+        <v>-0.03844888072395628</v>
       </c>
     </row>
   </sheetData>
@@ -617,15 +664,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -639,175 +686,441 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>161.74</v>
+      </c>
+      <c r="C2">
+        <v>190.829</v>
+      </c>
+      <c r="D2">
+        <v>683.5</v>
+      </c>
+      <c r="E2">
+        <v>43.63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0.4125710786143765</v>
+      </c>
+      <c r="C3">
+        <v>0.1051647568216076</v>
+      </c>
+      <c r="D3">
+        <v>0.1162016562414957</v>
+      </c>
+      <c r="E3">
+        <v>0.4496339369911597</v>
+      </c>
+      <c r="F3">
+        <v>0.4387071395849826</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.1913962061821985</v>
+      </c>
+      <c r="C4">
+        <v>0.1384383400030983</v>
+      </c>
+      <c r="D4">
+        <v>0.1537827237197764</v>
+      </c>
+      <c r="E4">
+        <v>0.4133837821808794</v>
+      </c>
+      <c r="F4">
+        <v>0.1984301527883283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.03663250774093866</v>
+      </c>
+      <c r="C5">
+        <v>0.01916517398281346</v>
+      </c>
+      <c r="D5">
+        <v>0.02364912611467308</v>
+      </c>
+      <c r="E5">
+        <v>0.1708861513701687</v>
+      </c>
+      <c r="F5">
+        <v>0.0393745255355993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.598275154235423</v>
+      </c>
+      <c r="C6">
+        <v>-0.104956455941808</v>
+      </c>
+      <c r="D6">
+        <v>-0.2001417301867452</v>
+      </c>
+      <c r="E6">
+        <v>0.3558744450200944</v>
+      </c>
+      <c r="F6">
+        <v>-0.05249116119637225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2.130009561889286</v>
+      </c>
+      <c r="C7">
+        <v>1.688795061363862</v>
+      </c>
+      <c r="D7">
+        <v>0.7875659701474236</v>
+      </c>
+      <c r="E7">
+        <v>0.7185392133336488</v>
+      </c>
+      <c r="F7">
+        <v>1.470637836340662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>-0.2987394378838335</v>
+      </c>
+      <c r="C8">
+        <v>-0.2164023914099338</v>
+      </c>
+      <c r="D8">
+        <v>-0.2330685652914314</v>
+      </c>
+      <c r="E8">
+        <v>-0.6277538396676976</v>
+      </c>
+      <c r="F8">
+        <v>-0.2739424874468516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>-0.3477189828540558</v>
+      </c>
+      <c r="C9">
+        <v>-0.2942055566680685</v>
+      </c>
+      <c r="D9">
+        <v>-0.3365936289548448</v>
+      </c>
+      <c r="E9">
+        <v>-0.7782206877391473</v>
+      </c>
+      <c r="F9">
+        <v>-0.4006976862458502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>-0.3879245432106935</v>
+      </c>
+      <c r="C10">
+        <v>-0.3282155213525744</v>
+      </c>
+      <c r="D10">
+        <v>-0.3856759614299178</v>
+      </c>
+      <c r="E10">
+        <v>-0.8421750478496322</v>
+      </c>
+      <c r="F10">
+        <v>-0.4493092504794094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>-0.4199363508683768</v>
+      </c>
+      <c r="C11">
+        <v>-0.4444184409698536</v>
+      </c>
+      <c r="D11">
+        <v>-0.4699085402334512</v>
+      </c>
+      <c r="E11">
+        <v>-0.9182835465285266</v>
+      </c>
+      <c r="F11">
+        <v>-0.6079301828592278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B2">
-        <v>201.3</v>
+        <v>1617.4</v>
       </c>
       <c r="C2">
-        <v>254.7</v>
+        <v>1908.29</v>
       </c>
       <c r="D2">
-        <v>781.3</v>
+        <v>6835</v>
       </c>
       <c r="E2">
-        <v>36.55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>436.3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.1024503323377223</v>
+        <v>0.01650284314457506</v>
       </c>
       <c r="C3">
-        <v>0.1555260871349182</v>
+        <v>0.004206590272864303</v>
       </c>
       <c r="D3">
-        <v>0.07484330056426232</v>
+        <v>0.004648066249659829</v>
       </c>
       <c r="E3">
-        <v>-0.04056224298771838</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0.01798535747964639</v>
+      </c>
+      <c r="F3">
+        <v>0.0175482855833993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.2186677295657215</v>
+        <v>0.1210495894101895</v>
       </c>
       <c r="C4">
-        <v>0.1883107487344456</v>
+        <v>0.08755609398051847</v>
       </c>
       <c r="D4">
-        <v>0.2018205519692798</v>
+        <v>0.09726073434777897</v>
       </c>
       <c r="E4">
-        <v>0.4982137427276083</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.2614468598933012</v>
+      </c>
+      <c r="F4">
+        <v>0.1254982478532657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0478155759534275</v>
+        <v>0.001465300309637546</v>
       </c>
       <c r="C5">
-        <v>0.03546093808892752</v>
+        <v>0.0007666069593125384</v>
       </c>
       <c r="D5">
-        <v>0.04073153519718479</v>
+        <v>0.0009459650445869232</v>
       </c>
       <c r="E5">
-        <v>0.2482169334426515</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.00683544605480675</v>
+      </c>
+      <c r="F5">
+        <v>0.001574981021423972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>-0.1736236955280446</v>
+        <v>5.982751542354229</v>
       </c>
       <c r="C6">
-        <v>-0.5310272909960784</v>
+        <v>-1.04956455941808</v>
       </c>
       <c r="D6">
-        <v>-0.4348566222261216</v>
+        <v>-2.001417301867452</v>
       </c>
       <c r="E6">
-        <v>-0.7210069636931663</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>3.558744450200944</v>
+      </c>
+      <c r="F6">
+        <v>-0.5249116119637225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>1.355289324219858</v>
+        <v>21.30009561889285</v>
       </c>
       <c r="C7">
-        <v>5.926437800708015</v>
+        <v>16.88795061363862</v>
       </c>
       <c r="D7">
-        <v>6.508584345364187</v>
+        <v>7.875659701474236</v>
       </c>
       <c r="E7">
-        <v>6.518477693830253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>7.185392133336488</v>
+      </c>
+      <c r="F7">
+        <v>14.70637836340662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>-0.3781941758637406</v>
+        <v>-0.1889394101262612</v>
       </c>
       <c r="C8">
-        <v>-0.2745837792388978</v>
+        <v>-0.1368648895925294</v>
       </c>
       <c r="D8">
-        <v>-0.3230833799503321</v>
+        <v>-0.1474055034617177</v>
       </c>
       <c r="E8">
-        <v>-0.7697470141608774</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>-0.3970263886532165</v>
+      </c>
+      <c r="F8">
+        <v>-0.1732564416448271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>-0.4946414199591536</v>
+        <v>-0.2199167942991705</v>
       </c>
       <c r="C9">
-        <v>-0.4449247688439585</v>
+        <v>-0.1860719318697671</v>
       </c>
       <c r="D9">
-        <v>-0.4851979970527825</v>
+        <v>-0.212880502679782</v>
       </c>
       <c r="E9">
-        <v>-1.129989723414279</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>-0.4921899791036756</v>
+      </c>
+      <c r="F9">
+        <v>-0.2534234683392821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>-0.5761840175054853</v>
+        <v>-0.2453450233652399</v>
       </c>
       <c r="C10">
-        <v>-0.5300218158961246</v>
+        <v>-0.2075817221787528</v>
       </c>
       <c r="D10">
-        <v>-0.5789038476077093</v>
+        <v>-0.2439228953787581</v>
       </c>
       <c r="E10">
-        <v>-1.19026955100657</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>-0.5326382679532256</v>
+      </c>
+      <c r="F10">
+        <v>-0.284168121059607</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>-0.6988773857096181</v>
+        <v>-0.2655910682087396</v>
       </c>
       <c r="C11">
-        <v>-0.7882213344514727</v>
+        <v>-0.2810749015291655</v>
       </c>
       <c r="D11">
-        <v>-0.77059159541897</v>
+        <v>-0.2971962558205153</v>
       </c>
       <c r="E11">
-        <v>-1.964850981352499</v>
+        <v>-0.58077350897747</v>
+      </c>
+      <c r="F11">
+        <v>-0.3844888072395628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit: 2025-04-22 12:47:17
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -7,16 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Daily_Statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="Annual_Statistics" sheetId="2" r:id="rId2"/>
-    <sheet name="10Day_Statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="1DDay_Statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="3DDay_Statistics" sheetId="2" r:id="rId2"/>
+    <sheet name="5DDay_Statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="10DDay_Statistics" sheetId="4" r:id="rId4"/>
+    <sheet name="Annual_Statistics" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -64,16 +66,6 @@
   </si>
   <si>
     <t>ES 99%</t>
-  </si>
-  <si>
-    <t>Ticker
-AAPL    191.380951
-Name: 249, dtype: float64</t>
-  </si>
-  <si>
-    <t>Ticker
-AAPL    1913.809509
-Name: 249, dtype: float64</t>
   </si>
 </sst>
 </file>
@@ -473,8 +465,8 @@
       <c r="E2">
         <v>43.63</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
+      <c r="F2">
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -494,7 +486,7 @@
         <v>0.001798535747964639</v>
       </c>
       <c r="F3">
-        <v>0.00175482855833993</v>
+        <v>0.001754828878540431</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -514,7 +506,7 @@
         <v>0.02614468598933013</v>
       </c>
       <c r="F4">
-        <v>0.01254982478532658</v>
+        <v>0.0125498204560367</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -534,7 +526,7 @@
         <v>0.0006835446054806749</v>
       </c>
       <c r="F5">
-        <v>0.0001574981021423972</v>
+        <v>0.0001574979934787571</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -554,7 +546,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.05249116119637225</v>
+        <v>-0.05249258457463724</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -574,7 +566,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>1.470637836340662</v>
+        <v>1.470631875486821</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -594,7 +586,7 @@
         <v>-0.03970263886532165</v>
       </c>
       <c r="F8">
-        <v>-0.01732564416448271</v>
+        <v>-0.01732572902443588</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -614,7 +606,7 @@
         <v>-0.04921899791036756</v>
       </c>
       <c r="F9">
-        <v>-0.02534234683392821</v>
+        <v>-0.02534233246732107</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -634,7 +626,7 @@
         <v>-0.05326382679532255</v>
       </c>
       <c r="F10">
-        <v>-0.02841681210596071</v>
+        <v>-0.0284168086240753</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -654,7 +646,7 @@
         <v>-0.05807735089774701</v>
       </c>
       <c r="F11">
-        <v>-0.03844888072395628</v>
+        <v>-0.03844890822549991</v>
       </c>
     </row>
   </sheetData>
@@ -706,8 +698,8 @@
       <c r="E2">
         <v>43.63</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
+      <c r="F2">
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -715,19 +707,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.4125710786143765</v>
+        <v>0.004950852943372519</v>
       </c>
       <c r="C3">
-        <v>0.1051647568216076</v>
+        <v>0.001261977081859291</v>
       </c>
       <c r="D3">
-        <v>0.1162016562414957</v>
+        <v>0.001394419874897949</v>
       </c>
       <c r="E3">
-        <v>0.4496339369911597</v>
+        <v>0.005395607243893917</v>
       </c>
       <c r="F3">
-        <v>0.4387071395849826</v>
+        <v>0.005264486635621293</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -735,19 +727,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.1913962061821985</v>
+        <v>0.02096640390937998</v>
       </c>
       <c r="C4">
-        <v>0.1384383400030983</v>
+        <v>0.01516516032865335</v>
       </c>
       <c r="D4">
-        <v>0.1537827237197764</v>
+        <v>0.01684605334718126</v>
       </c>
       <c r="E4">
-        <v>0.4133837821808794</v>
+        <v>0.04528392448145396</v>
       </c>
       <c r="F4">
-        <v>0.1984301527883283</v>
+        <v>0.02173692665572277</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -755,19 +747,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.03663250774093866</v>
+        <v>0.0004395900928912639</v>
       </c>
       <c r="C5">
-        <v>0.01916517398281346</v>
+        <v>0.0002299820877937615</v>
       </c>
       <c r="D5">
-        <v>0.02364912611467308</v>
+        <v>0.0002837895133760769</v>
       </c>
       <c r="E5">
-        <v>0.1708861513701687</v>
+        <v>0.002050633816442025</v>
       </c>
       <c r="F5">
-        <v>0.0393745255355993</v>
+        <v>0.0004724939804362713</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -787,7 +779,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.05249116119637225</v>
+        <v>-0.05249258457463724</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -807,7 +799,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>1.470637836340662</v>
+        <v>1.470631875486821</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -815,19 +807,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>-0.2987394378838335</v>
+        <v>-0.0327252657890778</v>
       </c>
       <c r="C8">
-        <v>-0.2164023914099338</v>
+        <v>-0.02370569425465658</v>
       </c>
       <c r="D8">
-        <v>-0.2330685652914314</v>
+        <v>-0.02553138213109651</v>
       </c>
       <c r="E8">
-        <v>-0.6277538396676976</v>
+        <v>-0.06876698770929586</v>
       </c>
       <c r="F8">
-        <v>-0.2739424874468516</v>
+        <v>-0.0300090429484937</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -835,19 +827,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>-0.3477189828540558</v>
+        <v>-0.03809070611638368</v>
       </c>
       <c r="C9">
-        <v>-0.2942055566680685</v>
+        <v>-0.03222860398609311</v>
       </c>
       <c r="D9">
-        <v>-0.3365936289548448</v>
+        <v>-0.0368719846582185</v>
       </c>
       <c r="E9">
-        <v>-0.7782206877391473</v>
+        <v>-0.08524980507838301</v>
       </c>
       <c r="F9">
-        <v>-0.4006976862458502</v>
+        <v>-0.04389420741570244</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -855,19 +847,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>-0.3879245432106935</v>
+        <v>-0.04249500458527687</v>
       </c>
       <c r="C10">
-        <v>-0.3282155213525744</v>
+        <v>-0.0359542089536247</v>
       </c>
       <c r="D10">
-        <v>-0.3856759614299178</v>
+        <v>-0.04224868479253168</v>
       </c>
       <c r="E10">
-        <v>-0.8421750478496322</v>
+        <v>-0.09225565421504722</v>
       </c>
       <c r="F10">
-        <v>-0.4493092504794094</v>
+        <v>-0.04921935632585985</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -875,19 +867,19 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>-0.4199363508683768</v>
+        <v>-0.04600172241740282</v>
       </c>
       <c r="C11">
-        <v>-0.4444184409698536</v>
+        <v>-0.04868360101809338</v>
       </c>
       <c r="D11">
-        <v>-0.4699085402334512</v>
+        <v>-0.05147590149003702</v>
       </c>
       <c r="E11">
-        <v>-0.9182835465285266</v>
+        <v>-0.1005929225239038</v>
       </c>
       <c r="F11">
-        <v>-0.6079301828592278</v>
+        <v>-0.06659546254211876</v>
       </c>
     </row>
   </sheetData>
@@ -928,19 +920,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>1617.4</v>
+        <v>161.74</v>
       </c>
       <c r="C2">
-        <v>1908.29</v>
+        <v>190.829</v>
       </c>
       <c r="D2">
-        <v>6835</v>
+        <v>683.5</v>
       </c>
       <c r="E2">
-        <v>436.3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
+        <v>43.63</v>
+      </c>
+      <c r="F2">
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -948,19 +940,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.01650284314457506</v>
+        <v>0.008251421572287532</v>
       </c>
       <c r="C3">
-        <v>0.004206590272864303</v>
+        <v>0.002103295136432151</v>
       </c>
       <c r="D3">
-        <v>0.004648066249659829</v>
+        <v>0.002324033124829915</v>
       </c>
       <c r="E3">
-        <v>0.01798535747964639</v>
+        <v>0.008992678739823195</v>
       </c>
       <c r="F3">
-        <v>0.0175482855833993</v>
+        <v>0.008774144392702155</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -968,19 +960,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.1210495894101895</v>
+        <v>0.02706751105696224</v>
       </c>
       <c r="C4">
-        <v>0.08755609398051847</v>
+        <v>0.01957813779847995</v>
       </c>
       <c r="D4">
-        <v>0.09726073434777897</v>
+        <v>0.02174816135431825</v>
       </c>
       <c r="E4">
-        <v>0.2614468598933012</v>
+        <v>0.0584612951225285</v>
       </c>
       <c r="F4">
-        <v>0.1254982478532657</v>
+        <v>0.02806225164511546</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -988,19 +980,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.001465300309637546</v>
+        <v>0.0007326501548187732</v>
       </c>
       <c r="C5">
-        <v>0.0007666069593125384</v>
+        <v>0.0003833034796562692</v>
       </c>
       <c r="D5">
-        <v>0.0009459650445869232</v>
+        <v>0.0004729825222934616</v>
       </c>
       <c r="E5">
-        <v>0.00683544605480675</v>
+        <v>0.003417723027403375</v>
       </c>
       <c r="F5">
-        <v>0.001574981021423972</v>
+        <v>0.0007874899673937855</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1008,19 +1000,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>5.982751542354229</v>
+        <v>0.598275154235423</v>
       </c>
       <c r="C6">
-        <v>-1.04956455941808</v>
+        <v>-0.104956455941808</v>
       </c>
       <c r="D6">
-        <v>-2.001417301867452</v>
+        <v>-0.2001417301867452</v>
       </c>
       <c r="E6">
-        <v>3.558744450200944</v>
+        <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.5249116119637225</v>
+        <v>-0.05249258457463724</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1028,19 +1020,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>21.30009561889285</v>
+        <v>2.130009561889286</v>
       </c>
       <c r="C7">
-        <v>16.88795061363862</v>
+        <v>1.688795061363862</v>
       </c>
       <c r="D7">
-        <v>7.875659701474236</v>
+        <v>0.7875659701474236</v>
       </c>
       <c r="E7">
-        <v>7.185392133336488</v>
+        <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>14.70637836340662</v>
+        <v>1.470631875486821</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1048,19 +1040,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>-0.1889394101262612</v>
+        <v>-0.04224813646710322</v>
       </c>
       <c r="C8">
-        <v>-0.1368648895925294</v>
+        <v>-0.03060391968618993</v>
       </c>
       <c r="D8">
-        <v>-0.1474055034617177</v>
+        <v>-0.03296087259979815</v>
       </c>
       <c r="E8">
-        <v>-0.3970263886532165</v>
+        <v>-0.08877779938898434</v>
       </c>
       <c r="F8">
-        <v>-0.1732564416448271</v>
+        <v>-0.03874150785837975</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1068,19 +1060,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>-0.2199167942991705</v>
+        <v>-0.04917489014467834</v>
       </c>
       <c r="C9">
-        <v>-0.1860719318697671</v>
+        <v>-0.04160694883655087</v>
       </c>
       <c r="D9">
-        <v>-0.212880502679782</v>
+        <v>-0.04760152750763189</v>
       </c>
       <c r="E9">
-        <v>-0.4921899791036756</v>
+        <v>-0.110057025112002</v>
       </c>
       <c r="F9">
-        <v>-0.2534234683392821</v>
+        <v>-0.05666717810532988</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1088,19 +1080,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>-0.2453450233652399</v>
+        <v>-0.05486081501859506</v>
       </c>
       <c r="C10">
-        <v>-0.2075817221787528</v>
+        <v>-0.04641668416781669</v>
       </c>
       <c r="D10">
-        <v>-0.2439228953787581</v>
+        <v>-0.05454281753354726</v>
       </c>
       <c r="E10">
-        <v>-0.5326382679532256</v>
+        <v>-0.119101537456116</v>
       </c>
       <c r="F10">
-        <v>-0.284168121059607</v>
+        <v>-0.06354191578703464</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1108,19 +1100,485 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>-0.2655910682087396</v>
+        <v>-0.05938796827315251</v>
       </c>
       <c r="C11">
-        <v>-0.2810749015291655</v>
+        <v>-0.06285025865882737</v>
       </c>
       <c r="D11">
-        <v>-0.2971962558205153</v>
+        <v>-0.06645510306730899</v>
       </c>
       <c r="E11">
-        <v>-0.58077350897747</v>
+        <v>-0.1298649045604708</v>
       </c>
       <c r="F11">
-        <v>-0.3844888072395628</v>
+        <v>-0.08597437245286861</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>161.74</v>
+      </c>
+      <c r="C2">
+        <v>190.829</v>
+      </c>
+      <c r="D2">
+        <v>683.5</v>
+      </c>
+      <c r="E2">
+        <v>43.63</v>
+      </c>
+      <c r="F2">
+        <v>191.3809661865234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0.01650284314457506</v>
+      </c>
+      <c r="C3">
+        <v>0.004206590272864303</v>
+      </c>
+      <c r="D3">
+        <v>0.004648066249659829</v>
+      </c>
+      <c r="E3">
+        <v>0.01798535747964639</v>
+      </c>
+      <c r="F3">
+        <v>0.01754828878540431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.03827924123643971</v>
+      </c>
+      <c r="C4">
+        <v>0.02768766800061967</v>
+      </c>
+      <c r="D4">
+        <v>0.03075654474395528</v>
+      </c>
+      <c r="E4">
+        <v>0.08267675643617589</v>
+      </c>
+      <c r="F4">
+        <v>0.03968601686724899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.001465300309637546</v>
+      </c>
+      <c r="C5">
+        <v>0.0007666069593125384</v>
+      </c>
+      <c r="D5">
+        <v>0.0009459650445869232</v>
+      </c>
+      <c r="E5">
+        <v>0.00683544605480675</v>
+      </c>
+      <c r="F5">
+        <v>0.001574979934787571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.598275154235423</v>
+      </c>
+      <c r="C6">
+        <v>-0.104956455941808</v>
+      </c>
+      <c r="D6">
+        <v>-0.2001417301867452</v>
+      </c>
+      <c r="E6">
+        <v>0.3558744450200944</v>
+      </c>
+      <c r="F6">
+        <v>-0.05249258457463724</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2.130009561889286</v>
+      </c>
+      <c r="C7">
+        <v>1.688795061363862</v>
+      </c>
+      <c r="D7">
+        <v>0.7875659701474236</v>
+      </c>
+      <c r="E7">
+        <v>0.7185392133336488</v>
+      </c>
+      <c r="F7">
+        <v>1.470631875486821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>-0.05974788757676671</v>
+      </c>
+      <c r="C8">
+        <v>-0.04328047828198676</v>
+      </c>
+      <c r="D8">
+        <v>-0.04661371305828628</v>
+      </c>
+      <c r="E8">
+        <v>-0.1255507679335395</v>
+      </c>
+      <c r="F8">
+        <v>-0.05478876584010448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>-0.06954379657081117</v>
+      </c>
+      <c r="C9">
+        <v>-0.05884111133361371</v>
+      </c>
+      <c r="D9">
+        <v>-0.06731872579096897</v>
+      </c>
+      <c r="E9">
+        <v>-0.1556441375478295</v>
+      </c>
+      <c r="F9">
+        <v>-0.08013949181796923</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>-0.07758490864213871</v>
+      </c>
+      <c r="C10">
+        <v>-0.06564310427051488</v>
+      </c>
+      <c r="D10">
+        <v>-0.07713519228598358</v>
+      </c>
+      <c r="E10">
+        <v>-0.1684350095699264</v>
+      </c>
+      <c r="F10">
+        <v>-0.08986183908519346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>-0.08398727017367535</v>
+      </c>
+      <c r="C11">
+        <v>-0.08888368819397073</v>
+      </c>
+      <c r="D11">
+        <v>-0.09398170804669025</v>
+      </c>
+      <c r="E11">
+        <v>-0.1836567093057054</v>
+      </c>
+      <c r="F11">
+        <v>-0.1215861235393626</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>161.74</v>
+      </c>
+      <c r="C2">
+        <v>190.829</v>
+      </c>
+      <c r="D2">
+        <v>683.5</v>
+      </c>
+      <c r="E2">
+        <v>43.63</v>
+      </c>
+      <c r="F2">
+        <v>191.3809661865234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0.4125710786143765</v>
+      </c>
+      <c r="C3">
+        <v>0.1051647568216076</v>
+      </c>
+      <c r="D3">
+        <v>0.1162016562414957</v>
+      </c>
+      <c r="E3">
+        <v>0.4496339369911597</v>
+      </c>
+      <c r="F3">
+        <v>0.4387072196351078</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.1913962061821985</v>
+      </c>
+      <c r="C4">
+        <v>0.1384383400030983</v>
+      </c>
+      <c r="D4">
+        <v>0.1537827237197764</v>
+      </c>
+      <c r="E4">
+        <v>0.4133837821808794</v>
+      </c>
+      <c r="F4">
+        <v>0.1984300843362449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.03663250774093866</v>
+      </c>
+      <c r="C5">
+        <v>0.01916517398281346</v>
+      </c>
+      <c r="D5">
+        <v>0.02364912611467308</v>
+      </c>
+      <c r="E5">
+        <v>0.1708861513701687</v>
+      </c>
+      <c r="F5">
+        <v>0.03937449836968927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.598275154235423</v>
+      </c>
+      <c r="C6">
+        <v>-0.104956455941808</v>
+      </c>
+      <c r="D6">
+        <v>-0.2001417301867452</v>
+      </c>
+      <c r="E6">
+        <v>0.3558744450200944</v>
+      </c>
+      <c r="F6">
+        <v>-0.05249258457463724</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2.130009561889286</v>
+      </c>
+      <c r="C7">
+        <v>1.688795061363862</v>
+      </c>
+      <c r="D7">
+        <v>0.7875659701474236</v>
+      </c>
+      <c r="E7">
+        <v>0.7185392133336488</v>
+      </c>
+      <c r="F7">
+        <v>1.470631875486821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>-0.2987394378838335</v>
+      </c>
+      <c r="C8">
+        <v>-0.2164023914099338</v>
+      </c>
+      <c r="D8">
+        <v>-0.2330685652914314</v>
+      </c>
+      <c r="E8">
+        <v>-0.6277538396676976</v>
+      </c>
+      <c r="F8">
+        <v>-0.2739438292005224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>-0.3477189828540558</v>
+      </c>
+      <c r="C9">
+        <v>-0.2942055566680685</v>
+      </c>
+      <c r="D9">
+        <v>-0.3365936289548448</v>
+      </c>
+      <c r="E9">
+        <v>-0.7782206877391473</v>
+      </c>
+      <c r="F9">
+        <v>-0.4006974590898461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>-0.3879245432106935</v>
+      </c>
+      <c r="C10">
+        <v>-0.3282155213525744</v>
+      </c>
+      <c r="D10">
+        <v>-0.3856759614299178</v>
+      </c>
+      <c r="E10">
+        <v>-0.8421750478496322</v>
+      </c>
+      <c r="F10">
+        <v>-0.4493091954259673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>-0.4199363508683768</v>
+      </c>
+      <c r="C11">
+        <v>-0.4444184409698536</v>
+      </c>
+      <c r="D11">
+        <v>-0.4699085402334512</v>
+      </c>
+      <c r="E11">
+        <v>-0.9182835465285266</v>
+      </c>
+      <c r="F11">
+        <v>-0.607930617696813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit: 2025-04-22 12:51:12
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="1DDay_Statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="3DDay_Statistics" sheetId="2" r:id="rId2"/>
-    <sheet name="5DDay_Statistics" sheetId="3" r:id="rId3"/>
-    <sheet name="10DDay_Statistics" sheetId="4" r:id="rId4"/>
+    <sheet name="1D_Statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="3D_Statistics" sheetId="2" r:id="rId2"/>
+    <sheet name="5D_Statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="10D_Statistics" sheetId="4" r:id="rId4"/>
     <sheet name="Annual_Statistics" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -486,7 +486,7 @@
         <v>0.001798535747964639</v>
       </c>
       <c r="F3">
-        <v>0.001754828878540431</v>
+        <v>0.001754828878540432</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -506,7 +506,7 @@
         <v>0.02614468598933013</v>
       </c>
       <c r="F4">
-        <v>0.0125498204560367</v>
+        <v>0.01254982721302963</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -526,7 +526,7 @@
         <v>0.0006835446054806749</v>
       </c>
       <c r="F5">
-        <v>0.0001574979934787571</v>
+        <v>0.000157498163076899</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -546,7 +546,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.05249258457463724</v>
+        <v>-0.05249309071118011</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -566,7 +566,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>1.470631875486821</v>
+        <v>1.470640435624273</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -586,7 +586,7 @@
         <v>-0.03970263886532165</v>
       </c>
       <c r="F8">
-        <v>-0.01732572902443588</v>
+        <v>-0.01732573067276034</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -606,7 +606,7 @@
         <v>-0.04921899791036756</v>
       </c>
       <c r="F9">
-        <v>-0.02534233246732107</v>
+        <v>-0.02534237462518862</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -626,7 +626,7 @@
         <v>-0.05326382679532255</v>
       </c>
       <c r="F10">
-        <v>-0.0284168086240753</v>
+        <v>-0.02841681823381926</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -646,7 +646,7 @@
         <v>-0.05807735089774701</v>
       </c>
       <c r="F11">
-        <v>-0.03844890822549991</v>
+        <v>-0.03844888055246375</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +719,7 @@
         <v>0.005395607243893917</v>
       </c>
       <c r="F3">
-        <v>0.005264486635621293</v>
+        <v>0.005264486635621296</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -739,7 +739,7 @@
         <v>0.04528392448145396</v>
       </c>
       <c r="F4">
-        <v>0.02173692665572277</v>
+        <v>0.02173693835917784</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -759,7 +759,7 @@
         <v>0.002050633816442025</v>
       </c>
       <c r="F5">
-        <v>0.0004724939804362713</v>
+        <v>0.0004724944892306971</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -779,7 +779,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.05249258457463724</v>
+        <v>-0.05249309071118011</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -799,7 +799,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>1.470631875486821</v>
+        <v>1.470640435624273</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -819,7 +819,7 @@
         <v>-0.06876698770929586</v>
       </c>
       <c r="F8">
-        <v>-0.0300090429484937</v>
+        <v>-0.03000904580347542</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -839,7 +839,7 @@
         <v>-0.08524980507838301</v>
       </c>
       <c r="F9">
-        <v>-0.04389420741570244</v>
+        <v>-0.04389428043527098</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -859,7 +859,7 @@
         <v>-0.09225565421504722</v>
       </c>
       <c r="F10">
-        <v>-0.04921935632585985</v>
+        <v>-0.04921937297042464</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -879,7 +879,7 @@
         <v>-0.1005929225239038</v>
       </c>
       <c r="F11">
-        <v>-0.06659546254211876</v>
+        <v>-0.06659541461101413</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +952,7 @@
         <v>0.008992678739823195</v>
       </c>
       <c r="F3">
-        <v>0.008774144392702155</v>
+        <v>0.00877414439270216</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -972,7 +972,7 @@
         <v>0.0584612951225285</v>
       </c>
       <c r="F4">
-        <v>0.02806225164511546</v>
+        <v>0.02806226675421099</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -992,7 +992,7 @@
         <v>0.003417723027403375</v>
       </c>
       <c r="F5">
-        <v>0.0007874899673937855</v>
+        <v>0.0007874908153844952</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1012,7 +1012,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.05249258457463724</v>
+        <v>-0.05249309071118011</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1032,7 +1032,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>1.470631875486821</v>
+        <v>1.470640435624273</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1052,7 +1052,7 @@
         <v>-0.08877779938898434</v>
       </c>
       <c r="F8">
-        <v>-0.03874150785837975</v>
+        <v>-0.03874151154414529</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1072,7 +1072,7 @@
         <v>-0.110057025112002</v>
       </c>
       <c r="F9">
-        <v>-0.05666717810532988</v>
+        <v>-0.05666727237318752</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1092,7 +1092,7 @@
         <v>-0.119101537456116</v>
       </c>
       <c r="F10">
-        <v>-0.06354191578703464</v>
+        <v>-0.06354193727507539</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1112,7 +1112,7 @@
         <v>-0.1298649045604708</v>
       </c>
       <c r="F11">
-        <v>-0.08597437245286861</v>
+        <v>-0.08597431057407863</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1185,7 @@
         <v>0.01798535747964639</v>
       </c>
       <c r="F3">
-        <v>0.01754828878540431</v>
+        <v>0.01754828878540432</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1205,7 +1205,7 @@
         <v>0.08267675643617589</v>
       </c>
       <c r="F4">
-        <v>0.03968601686724899</v>
+        <v>0.03968603823473679</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1225,7 +1225,7 @@
         <v>0.00683544605480675</v>
       </c>
       <c r="F5">
-        <v>0.001574979934787571</v>
+        <v>0.00157498163076899</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1245,7 +1245,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.05249258457463724</v>
+        <v>-0.05249309071118011</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1265,7 +1265,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>1.470631875486821</v>
+        <v>1.470640435624273</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1285,7 +1285,7 @@
         <v>-0.1255507679335395</v>
       </c>
       <c r="F8">
-        <v>-0.05478876584010448</v>
+        <v>-0.0547887710525641</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1305,7 +1305,7 @@
         <v>-0.1556441375478295</v>
       </c>
       <c r="F9">
-        <v>-0.08013949181796923</v>
+        <v>-0.080139625132852</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1325,7 +1325,7 @@
         <v>-0.1684350095699264</v>
       </c>
       <c r="F10">
-        <v>-0.08986183908519346</v>
+        <v>-0.08986186947387211</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1345,7 +1345,7 @@
         <v>-0.1836567093057054</v>
       </c>
       <c r="F11">
-        <v>-0.1215861235393626</v>
+        <v>-0.1215860360295386</v>
       </c>
     </row>
   </sheetData>
@@ -1418,7 +1418,7 @@
         <v>0.4496339369911597</v>
       </c>
       <c r="F3">
-        <v>0.4387072196351078</v>
+        <v>0.438707219635108</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1438,7 +1438,7 @@
         <v>0.4133837821808794</v>
       </c>
       <c r="F4">
-        <v>0.1984300843362449</v>
+        <v>0.198430191173684</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1458,7 +1458,7 @@
         <v>0.1708861513701687</v>
       </c>
       <c r="F5">
-        <v>0.03937449836968927</v>
+        <v>0.03937454076922476</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1478,7 +1478,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6">
-        <v>-0.05249258457463724</v>
+        <v>-0.05249309071118011</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1498,7 +1498,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7">
-        <v>1.470631875486821</v>
+        <v>1.470640435624273</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1518,7 +1518,7 @@
         <v>-0.6277538396676976</v>
       </c>
       <c r="F8">
-        <v>-0.2739438292005224</v>
+        <v>-0.2739438552628204</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1538,7 +1538,7 @@
         <v>-0.7782206877391473</v>
       </c>
       <c r="F9">
-        <v>-0.4006974590898461</v>
+        <v>-0.4006981256642599</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1558,7 +1558,7 @@
         <v>-0.8421750478496322</v>
       </c>
       <c r="F10">
-        <v>-0.4493091954259673</v>
+        <v>-0.4493093473693605</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1578,7 +1578,7 @@
         <v>-0.9182835465285266</v>
       </c>
       <c r="F11">
-        <v>-0.607930617696813</v>
+        <v>-0.6079301801476928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit: 2025-04-22 13:04:23
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -72,6 +72,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -124,11 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,6 +434,10 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -453,19 +463,19 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>161.74</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>190.829</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>683.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>43.63</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>191.3809661865234</v>
       </c>
     </row>
@@ -473,180 +483,180 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.001650284314457506</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.0004206590272864303</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.0004648066249659829</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0.001798535747964639</v>
       </c>
-      <c r="F3">
-        <v>0.001754828878540432</v>
+      <c r="F3" s="3">
+        <v>0.001754828630708089</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.01210495894101895</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.008755609398051848</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.009726073434777898</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0.02614468598933013</v>
       </c>
-      <c r="F4">
-        <v>0.01254982721302963</v>
+      <c r="F4" s="3">
+        <v>0.01254981569492755</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.0001465300309637546</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>7.666069593125384E-05</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>9.459650445869232E-05</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.0006835446054806749</v>
       </c>
-      <c r="F5">
-        <v>0.000157498163076899</v>
+      <c r="F5" s="3">
+        <v>0.00015749787397665</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.598275154235423</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>-0.104956455941808</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>-0.2001417301867452</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.3558744450200944</v>
       </c>
-      <c r="F6">
-        <v>-0.05249309071118011</v>
+      <c r="F6" s="3">
+        <v>-0.05248831627412358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>2.130009561889286</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1.688795061363862</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.7875659701474236</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.7185392133336488</v>
       </c>
-      <c r="F7">
-        <v>1.470640435624273</v>
+      <c r="F7" s="3">
+        <v>1.470639256666352</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-0.01889394101262612</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>-0.01368648895925294</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>-0.01474055034617178</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>-0.03970263886532165</v>
       </c>
-      <c r="F8">
-        <v>-0.01732573067276034</v>
+      <c r="F8" s="3">
+        <v>-0.01732566152014103</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>-0.02199167942991705</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>-0.01860719318697671</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>-0.0212880502679782</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>-0.04921899791036756</v>
       </c>
-      <c r="F9">
-        <v>-0.02534237462518862</v>
+      <c r="F9" s="3">
+        <v>-0.02534230624938148</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>-0.02453450233652399</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>-0.02075817221787528</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>-0.02439228953787581</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>-0.05326382679532255</v>
       </c>
-      <c r="F10">
-        <v>-0.02841681823381926</v>
+      <c r="F10" s="3">
+        <v>-0.02841681343529507</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>-0.02655910682087396</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>-0.02810749015291655</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>-0.02971962558205153</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>-0.05807735089774701</v>
       </c>
-      <c r="F11">
-        <v>-0.03844888055246375</v>
+      <c r="F11" s="3">
+        <v>-0.03844882687813962</v>
       </c>
     </row>
   </sheetData>
@@ -661,6 +671,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -686,19 +700,19 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>161.74</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>190.829</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>683.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>43.63</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>191.3809661865234</v>
       </c>
     </row>
@@ -706,180 +720,180 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.004950852943372519</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.001261977081859291</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.001394419874897949</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0.005395607243893917</v>
       </c>
-      <c r="F3">
-        <v>0.005264486635621296</v>
+      <c r="F3" s="3">
+        <v>0.005264485892124266</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.02096640390937998</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.01516516032865335</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.01684605334718126</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0.04528392448145396</v>
       </c>
-      <c r="F4">
-        <v>0.02173693835917784</v>
+      <c r="F4" s="3">
+        <v>0.02173691840923984</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.0004395900928912639</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.0002299820877937615</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.0002837895133760769</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.002050633816442025</v>
       </c>
-      <c r="F5">
-        <v>0.0004724944892306971</v>
+      <c r="F5" s="3">
+        <v>0.0004724936219299499</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.598275154235423</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>-0.104956455941808</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>-0.2001417301867452</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.3558744450200944</v>
       </c>
-      <c r="F6">
-        <v>-0.05249309071118011</v>
+      <c r="F6" s="3">
+        <v>-0.05248831627412358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>2.130009561889286</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1.688795061363862</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.7875659701474236</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.7185392133336488</v>
       </c>
-      <c r="F7">
-        <v>1.470640435624273</v>
+      <c r="F7" s="3">
+        <v>1.470639256666352</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-0.0327252657890778</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>-0.02370569425465658</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>-0.02553138213109651</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>-0.06876698770929586</v>
       </c>
-      <c r="F8">
-        <v>-0.03000904580347542</v>
+      <c r="F8" s="3">
+        <v>-0.03000892602762529</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>-0.03809070611638368</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>-0.03222860398609311</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>-0.0368719846582185</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>-0.08524980507838301</v>
       </c>
-      <c r="F9">
-        <v>-0.04389428043527098</v>
+      <c r="F9" s="3">
+        <v>-0.04389416200489899</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>-0.04249500458527687</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>-0.0359542089536247</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>-0.04224868479253168</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>-0.09225565421504722</v>
       </c>
-      <c r="F10">
-        <v>-0.04921937297042464</v>
+      <c r="F10" s="3">
+        <v>-0.04921936465913694</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>-0.04600172241740282</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>-0.04868360101809338</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>-0.05147590149003702</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>-0.1005929225239038</v>
       </c>
-      <c r="F11">
-        <v>-0.06659541461101413</v>
+      <c r="F11" s="3">
+        <v>-0.06659532164435768</v>
       </c>
     </row>
   </sheetData>
@@ -894,6 +908,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -919,19 +937,19 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>161.74</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>190.829</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>683.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>43.63</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>191.3809661865234</v>
       </c>
     </row>
@@ -939,180 +957,180 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.008251421572287532</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.002103295136432151</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.002324033124829915</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0.008992678739823195</v>
       </c>
-      <c r="F3">
-        <v>0.00877414439270216</v>
+      <c r="F3" s="3">
+        <v>0.008774143153540442</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.02706751105696224</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.01957813779847995</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.02174816135431825</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0.0584612951225285</v>
       </c>
-      <c r="F4">
-        <v>0.02806226675421099</v>
+      <c r="F4" s="3">
+        <v>0.02806224099895177</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.0007326501548187732</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.0003833034796562692</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.0004729825222934616</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.003417723027403375</v>
       </c>
-      <c r="F5">
-        <v>0.0007874908153844952</v>
+      <c r="F5" s="3">
+        <v>0.0007874893698832498</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.598275154235423</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>-0.104956455941808</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>-0.2001417301867452</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.3558744450200944</v>
       </c>
-      <c r="F6">
-        <v>-0.05249309071118011</v>
+      <c r="F6" s="3">
+        <v>-0.05248831627412358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>2.130009561889286</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1.688795061363862</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.7875659701474236</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.7185392133336488</v>
       </c>
-      <c r="F7">
-        <v>1.470640435624273</v>
+      <c r="F7" s="3">
+        <v>1.470639256666352</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-0.04224813646710322</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>-0.03060391968618993</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>-0.03296087259979815</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>-0.08877779938898434</v>
       </c>
-      <c r="F8">
-        <v>-0.03874151154414529</v>
+      <c r="F8" s="3">
+        <v>-0.03874135691418769</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>-0.04917489014467834</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>-0.04160694883655087</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>-0.04760152750763189</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>-0.110057025112002</v>
       </c>
-      <c r="F9">
-        <v>-0.05666727237318752</v>
+      <c r="F9" s="3">
+        <v>-0.05666711948023473</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>-0.05486081501859506</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>-0.04641668416781669</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>-0.05454281753354726</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>-0.119101537456116</v>
       </c>
-      <c r="F10">
-        <v>-0.06354193727507539</v>
+      <c r="F10" s="3">
+        <v>-0.06354192654524909</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>-0.05938796827315251</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>-0.06285025865882737</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>-0.06645510306730899</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>-0.1298649045604708</v>
       </c>
-      <c r="F11">
-        <v>-0.08597431057407863</v>
+      <c r="F11" s="3">
+        <v>-0.0859741905546412</v>
       </c>
     </row>
   </sheetData>
@@ -1127,6 +1145,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -1152,19 +1174,19 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>161.74</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>190.829</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>683.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>43.63</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>191.3809661865234</v>
       </c>
     </row>
@@ -1172,180 +1194,180 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.01650284314457506</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.004206590272864303</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.004648066249659829</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0.01798535747964639</v>
       </c>
-      <c r="F3">
-        <v>0.01754828878540432</v>
+      <c r="F3" s="3">
+        <v>0.01754828630708088</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.03827924123643971</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.02768766800061967</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.03075654474395528</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0.08267675643617589</v>
       </c>
-      <c r="F4">
-        <v>0.03968603823473679</v>
+      <c r="F4" s="3">
+        <v>0.03968600181129991</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.001465300309637546</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.0007666069593125384</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.0009459650445869232</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.00683544605480675</v>
       </c>
-      <c r="F5">
-        <v>0.00157498163076899</v>
+      <c r="F5" s="3">
+        <v>0.0015749787397665</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.598275154235423</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>-0.104956455941808</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>-0.2001417301867452</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.3558744450200944</v>
       </c>
-      <c r="F6">
-        <v>-0.05249309071118011</v>
+      <c r="F6" s="3">
+        <v>-0.05248831627412358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>2.130009561889286</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1.688795061363862</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.7875659701474236</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.7185392133336488</v>
       </c>
-      <c r="F7">
-        <v>1.470640435624273</v>
+      <c r="F7" s="3">
+        <v>1.470639256666352</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-0.05974788757676671</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>-0.04328047828198676</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>-0.04661371305828628</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>-0.1255507679335395</v>
       </c>
-      <c r="F8">
-        <v>-0.0547887710525641</v>
+      <c r="F8" s="3">
+        <v>-0.05478855237278091</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>-0.06954379657081117</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>-0.05884111133361371</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>-0.06731872579096897</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>-0.1556441375478295</v>
       </c>
-      <c r="F9">
-        <v>-0.080139625132852</v>
+      <c r="F9" s="3">
+        <v>-0.08013940890956457</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>-0.07758490864213871</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>-0.06564310427051488</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>-0.07713519228598358</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>-0.1684350095699264</v>
       </c>
-      <c r="F10">
-        <v>-0.08986186947387211</v>
+      <c r="F10" s="3">
+        <v>-0.08986185429960625</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>-0.08398727017367535</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>-0.08888368819397073</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>-0.09398170804669025</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>-0.1836567093057054</v>
       </c>
-      <c r="F11">
-        <v>-0.1215860360295386</v>
+      <c r="F11" s="3">
+        <v>-0.1215858662964224</v>
       </c>
     </row>
   </sheetData>
@@ -1360,6 +1382,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -1385,19 +1411,19 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>161.74</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>190.829</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>683.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>43.63</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>191.3809661865234</v>
       </c>
     </row>
@@ -1405,180 +1431,180 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.4125710786143765</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.1051647568216076</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.1162016562414957</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0.4496339369911597</v>
       </c>
-      <c r="F3">
-        <v>0.438707219635108</v>
+      <c r="F3" s="3">
+        <v>0.4387071576770221</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.1913962061821985</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.1384383400030983</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.1537827237197764</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0.4133837821808794</v>
       </c>
-      <c r="F4">
-        <v>0.198430191173684</v>
+      <c r="F4" s="3">
+        <v>0.1984300090564995</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.03663250774093866</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.01916517398281346</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.02364912611467308</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.1708861513701687</v>
       </c>
-      <c r="F5">
-        <v>0.03937454076922476</v>
+      <c r="F5" s="3">
+        <v>0.03937446849416249</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.598275154235423</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>-0.104956455941808</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>-0.2001417301867452</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.3558744450200944</v>
       </c>
-      <c r="F6">
-        <v>-0.05249309071118011</v>
+      <c r="F6" s="3">
+        <v>-0.05248831627412358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>2.130009561889286</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1.688795061363862</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.7875659701474236</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.7185392133336488</v>
       </c>
-      <c r="F7">
-        <v>1.470640435624273</v>
+      <c r="F7" s="3">
+        <v>1.470639256666352</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-0.2987394378838335</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>-0.2164023914099338</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>-0.2330685652914314</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>-0.6277538396676976</v>
       </c>
-      <c r="F8">
-        <v>-0.2739438552628204</v>
+      <c r="F8" s="3">
+        <v>-0.2739427618639045</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>-0.3477189828540558</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>-0.2942055566680685</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>-0.3365936289548448</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>-0.7782206877391473</v>
       </c>
-      <c r="F9">
-        <v>-0.4006981256642599</v>
+      <c r="F9" s="3">
+        <v>-0.4006970445478228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>-0.3879245432106935</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>-0.3282155213525744</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>-0.3856759614299178</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>-0.8421750478496322</v>
       </c>
-      <c r="F10">
-        <v>-0.4493093473693605</v>
+      <c r="F10" s="3">
+        <v>-0.4493092714980312</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>-0.4199363508683768</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>-0.4444184409698536</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>-0.4699085402334512</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>-0.9182835465285266</v>
       </c>
-      <c r="F11">
-        <v>-0.6079301801476928</v>
+      <c r="F11" s="3">
+        <v>-0.6079293314821121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit: 2025-04-22 13:48:26
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -66,6 +66,25 @@
   </si>
   <si>
     <t>ES 99%</t>
+  </si>
+  <si>
+    <t>CAGR</t>
+  </si>
+  <si>
+    <t>Max Drawdown</t>
+  </si>
+  <si>
+    <t>Calmar Ratio</t>
+  </si>
+  <si>
+    <t>Ticker
+AAPL    0.543144
+dtype: float64</t>
+  </si>
+  <si>
+    <t>Ticker
+AAPL    3.637364
+dtype: float64</t>
   </si>
 </sst>
 </file>
@@ -429,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -476,7 +495,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809661865234</v>
+        <v>191.3809509277344</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -496,7 +515,7 @@
         <v>0.001798535747964639</v>
       </c>
       <c r="F3" s="3">
-        <v>0.001754828630708089</v>
+        <v>0.001754828062675263</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -516,7 +535,7 @@
         <v>0.02614468598933013</v>
       </c>
       <c r="F4" s="3">
-        <v>0.01254981569492755</v>
+        <v>0.01254982252972077</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -536,7 +555,7 @@
         <v>0.0006835446054806749</v>
       </c>
       <c r="F5" s="3">
-        <v>0.00015749787397665</v>
+        <v>0.0001574980455274869</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -556,7 +575,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05248831627412358</v>
+        <v>-0.05249051910732176</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -576,7 +595,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470639256666352</v>
+        <v>1.470629158572999</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -596,7 +615,7 @@
         <v>-0.03970263886532165</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.01732566152014103</v>
+        <v>-0.01732569579896578</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -616,7 +635,7 @@
         <v>-0.04921899791036756</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.02534230624938148</v>
+        <v>-0.0253423453272444</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -636,7 +655,7 @@
         <v>-0.05326382679532255</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.02841681343529507</v>
+        <v>-0.02841676709174202</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -656,7 +675,67 @@
         <v>-0.05807735089774701</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.03844882687813962</v>
+        <v>-0.03844882503152471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5257815340198895</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1165552785803567</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.104274499922256</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5210181173153532</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.5431444910556542</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.1039095986491753</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.09780922394543157</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.1303597122302159</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.2793225480283115</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-0.1493236606462561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.059990038023909</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.191659374021654</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.799898205805385</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.865292010949807</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.637363889319251</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +745,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -713,7 +792,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809661865234</v>
+        <v>191.3809509277344</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -733,7 +812,7 @@
         <v>0.005395607243893917</v>
       </c>
       <c r="F3" s="3">
-        <v>0.005264485892124266</v>
+        <v>0.00526448418802579</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -753,7 +832,7 @@
         <v>0.04528392448145396</v>
       </c>
       <c r="F4" s="3">
-        <v>0.02173691840923984</v>
+        <v>0.02173693024744894</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -773,7 +852,7 @@
         <v>0.002050633816442025</v>
       </c>
       <c r="F5" s="3">
-        <v>0.0004724936219299499</v>
+        <v>0.0004724941365824608</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -793,7 +872,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05248831627412358</v>
+        <v>-0.05249051910732176</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -813,7 +892,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470639256666352</v>
+        <v>1.470629158572999</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -833,7 +912,7 @@
         <v>-0.06876698770929586</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.03000892602762529</v>
+        <v>-0.03000898540029139</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -853,7 +932,7 @@
         <v>-0.08524980507838301</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.04389416200489899</v>
+        <v>-0.04389422968974303</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -873,7 +952,7 @@
         <v>-0.09225565421504722</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.04921936465913694</v>
+        <v>-0.04921928438974845</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -893,7 +972,67 @@
         <v>-0.1005929225239038</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.06659532164435768</v>
+        <v>-0.06659531844592684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5257815340198895</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1165552785803567</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.104274499922256</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5210181173153532</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.5431444910556542</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.1039095986491753</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.09780922394543157</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.1303597122302159</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.2793225480283115</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-0.1493236606462561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.059990038023909</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.191659374021654</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.799898205805385</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.865292010949807</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.637363889319251</v>
       </c>
     </row>
   </sheetData>
@@ -903,7 +1042,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -950,7 +1089,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809661865234</v>
+        <v>191.3809509277344</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -970,7 +1109,7 @@
         <v>0.008992678739823195</v>
       </c>
       <c r="F3" s="3">
-        <v>0.008774143153540442</v>
+        <v>0.008774140313376318</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -990,7 +1129,7 @@
         <v>0.0584612951225285</v>
       </c>
       <c r="F4" s="3">
-        <v>0.02806224099895177</v>
+        <v>0.02806225628201401</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1010,7 +1149,7 @@
         <v>0.003417723027403375</v>
       </c>
       <c r="F5" s="3">
-        <v>0.0007874893698832498</v>
+        <v>0.0007874902276374348</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1030,7 +1169,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05248831627412358</v>
+        <v>-0.05249051910732176</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1050,7 +1189,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470639256666352</v>
+        <v>1.470629158572999</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1070,7 +1209,7 @@
         <v>-0.08877779938898434</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.03874135691418769</v>
+        <v>-0.03874143356397003</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1090,7 +1229,7 @@
         <v>-0.110057025112002</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.05666711948023473</v>
+        <v>-0.05666720686099264</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1110,7 +1249,7 @@
         <v>-0.119101537456116</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.06354192654524909</v>
+        <v>-0.06354182291791416</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1130,7 +1269,67 @@
         <v>-0.1298649045604708</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.0859741905546412</v>
+        <v>-0.08597418642548475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5257815340198895</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1165552785803567</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.104274499922256</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5210181173153532</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.5431444910556542</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.1039095986491753</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.09780922394543157</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.1303597122302159</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.2793225480283115</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-0.1493236606462561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.059990038023909</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.191659374021654</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.799898205805385</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.865292010949807</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.637363889319251</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1339,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1187,7 +1386,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809661865234</v>
+        <v>191.3809509277344</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1207,7 +1406,7 @@
         <v>0.01798535747964639</v>
       </c>
       <c r="F3" s="3">
-        <v>0.01754828630708088</v>
+        <v>0.01754828062675264</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1227,7 +1426,7 @@
         <v>0.08267675643617589</v>
       </c>
       <c r="F4" s="3">
-        <v>0.03968600181129991</v>
+        <v>0.0396860234248138</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1247,7 +1446,7 @@
         <v>0.00683544605480675</v>
       </c>
       <c r="F5" s="3">
-        <v>0.0015749787397665</v>
+        <v>0.00157498045527487</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1267,7 +1466,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05248831627412358</v>
+        <v>-0.05249051910732176</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1287,7 +1486,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470639256666352</v>
+        <v>1.470629158572999</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1307,7 +1506,7 @@
         <v>-0.1255507679335395</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.05478855237278091</v>
+        <v>-0.05478866077194264</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1327,7 +1526,7 @@
         <v>-0.1556441375478295</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.08013940890956457</v>
+        <v>-0.08013953248461748</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1347,7 +1546,7 @@
         <v>-0.1684350095699264</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.08986185429960625</v>
+        <v>-0.08986170774842375</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1367,7 +1566,67 @@
         <v>-0.1836567093057054</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.1215858662964224</v>
+        <v>-0.1215858604569134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5257815340198895</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1165552785803567</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.104274499922256</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5210181173153532</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.5431444910556542</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.1039095986491753</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.09780922394543157</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.1303597122302159</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.2793225480283115</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-0.1493236606462561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.059990038023909</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.191659374021654</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.799898205805385</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.865292010949807</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.637363889319251</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1636,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1424,7 +1683,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809661865234</v>
+        <v>191.3809509277344</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1444,7 +1703,7 @@
         <v>0.4496339369911597</v>
       </c>
       <c r="F3" s="3">
-        <v>0.4387071576770221</v>
+        <v>0.4387070156688158</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1464,7 +1723,7 @@
         <v>0.4133837821808794</v>
       </c>
       <c r="F4" s="3">
-        <v>0.1984300090564995</v>
+        <v>0.198430117124069</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1484,7 +1743,7 @@
         <v>0.1708861513701687</v>
       </c>
       <c r="F5" s="3">
-        <v>0.03937446849416249</v>
+        <v>0.03937451138187174</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1504,7 +1763,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05248831627412358</v>
+        <v>-0.05249051910732176</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1524,7 +1783,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470639256666352</v>
+        <v>1.470629158572999</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1544,7 +1803,7 @@
         <v>-0.6277538396676976</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.2739427618639045</v>
+        <v>-0.2739433038597132</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1564,7 +1823,7 @@
         <v>-0.7782206877391473</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.4006970445478228</v>
+        <v>-0.4006976624230874</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1584,7 +1843,7 @@
         <v>-0.8421750478496322</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.4493092714980312</v>
+        <v>-0.4493085387421187</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1604,7 +1863,67 @@
         <v>-0.9182835465285266</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.6079293314821121</v>
+        <v>-0.6079293022845669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5257815340198895</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1165552785803567</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.104274499922256</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5210181173153532</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.5431444910556542</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.1039095986491753</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.09780922394543157</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.1303597122302159</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.2793225480283115</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-0.1493236606462561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.059990038023909</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.191659374021654</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.799898205805385</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.865292010949807</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.637363889319251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit: 2025-04-22 14:03:43
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
+++ b/Pythonowe Analizy/Excels/portfolio_statistics.xlsx
@@ -11,14 +11,15 @@
     <sheet name="3D_Statistics" sheetId="2" r:id="rId2"/>
     <sheet name="5D_Statistics" sheetId="3" r:id="rId3"/>
     <sheet name="10D_Statistics" sheetId="4" r:id="rId4"/>
-    <sheet name="Annual_Statistics" sheetId="5" r:id="rId5"/>
+    <sheet name="1M_Statistics" sheetId="5" r:id="rId5"/>
+    <sheet name="Annual_Statistics" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
   <si>
     <t>NASDAQ</t>
   </si>
@@ -78,12 +79,12 @@
   </si>
   <si>
     <t>Ticker
-AAPL    0.543144
+AAPL    0.543145
 dtype: float64</t>
   </si>
   <si>
     <t>Ticker
-AAPL    3.637364
+AAPL    3.637365
 dtype: float64</t>
   </si>
 </sst>
@@ -495,7 +496,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809509277344</v>
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -515,7 +516,7 @@
         <v>0.001798535747964639</v>
       </c>
       <c r="F3" s="3">
-        <v>0.001754828062675263</v>
+        <v>0.001754828630708088</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -535,7 +536,7 @@
         <v>0.02614468598933013</v>
       </c>
       <c r="F4" s="3">
-        <v>0.01254982252972077</v>
+        <v>0.0125498100513117</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -555,7 +556,7 @@
         <v>0.0006835446054806749</v>
       </c>
       <c r="F5" s="3">
-        <v>0.0001574980455274869</v>
+        <v>0.0001574977323240041</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -575,7 +576,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05249051910732176</v>
+        <v>-0.05248821566458358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -595,7 +596,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470629158572999</v>
+        <v>1.470635920535974</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -635,7 +636,7 @@
         <v>-0.04921899791036756</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.0253423453272444</v>
+        <v>-0.02534225636928439</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -655,7 +656,7 @@
         <v>-0.05326382679532255</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.02841676709174202</v>
+        <v>-0.02841672472349273</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -675,7 +676,7 @@
         <v>-0.05807735089774701</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.03844882503152471</v>
+        <v>-0.03844879802287123</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -695,7 +696,7 @@
         <v>0.5210181173153532</v>
       </c>
       <c r="F12" s="3">
-        <v>0.5431444910556542</v>
+        <v>0.5431446161467421</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -735,7 +736,7 @@
         <v>1.865292010949807</v>
       </c>
       <c r="F14" s="3">
-        <v>3.637363889319251</v>
+        <v>3.637364727037048</v>
       </c>
     </row>
   </sheetData>
@@ -792,7 +793,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809509277344</v>
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -812,7 +813,7 @@
         <v>0.005395607243893917</v>
       </c>
       <c r="F3" s="3">
-        <v>0.00526448418802579</v>
+        <v>0.005264485892124264</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -832,7 +833,7 @@
         <v>0.04528392448145396</v>
       </c>
       <c r="F4" s="3">
-        <v>0.02173693024744894</v>
+        <v>0.02173690863421044</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -852,7 +853,7 @@
         <v>0.002050633816442025</v>
       </c>
       <c r="F5" s="3">
-        <v>0.0004724941365824608</v>
+        <v>0.0004724931969720122</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -872,7 +873,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05249051910732176</v>
+        <v>-0.05248821566458358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -892,7 +893,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470629158572999</v>
+        <v>1.470635920535974</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -932,7 +933,7 @@
         <v>-0.08524980507838301</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.04389422968974303</v>
+        <v>-0.04389407561003655</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -952,7 +953,7 @@
         <v>-0.09225565421504722</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.04921928438974845</v>
+        <v>-0.04921921100578806</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -972,7 +973,7 @@
         <v>-0.1005929225239038</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.06659531844592684</v>
+        <v>-0.06659527166556675</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -992,7 +993,7 @@
         <v>0.5210181173153532</v>
       </c>
       <c r="F12" s="3">
-        <v>0.5431444910556542</v>
+        <v>0.5431446161467421</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1032,7 +1033,7 @@
         <v>1.865292010949807</v>
       </c>
       <c r="F14" s="3">
-        <v>3.637363889319251</v>
+        <v>3.637364727037048</v>
       </c>
     </row>
   </sheetData>
@@ -1089,7 +1090,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809509277344</v>
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1109,7 +1110,7 @@
         <v>0.008992678739823195</v>
       </c>
       <c r="F3" s="3">
-        <v>0.008774140313376318</v>
+        <v>0.008774143153540439</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1129,7 +1130,7 @@
         <v>0.0584612951225285</v>
       </c>
       <c r="F4" s="3">
-        <v>0.02806225628201401</v>
+        <v>0.02806222837944308</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1149,7 +1150,7 @@
         <v>0.003417723027403375</v>
       </c>
       <c r="F5" s="3">
-        <v>0.0007874902276374348</v>
+        <v>0.0007874886616200204</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1169,7 +1170,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05249051910732176</v>
+        <v>-0.05248821566458358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1189,7 +1190,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470629158572999</v>
+        <v>1.470635920535974</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1229,7 +1230,7 @@
         <v>-0.110057025112002</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.05666720686099264</v>
+        <v>-0.05666700794494692</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1249,7 +1250,7 @@
         <v>-0.119101537456116</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.06354182291791416</v>
+        <v>-0.06354172817962866</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1269,7 +1270,7 @@
         <v>-0.1298649045604708</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.08597418642548475</v>
+        <v>-0.08597412603229958</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1289,7 +1290,7 @@
         <v>0.5210181173153532</v>
       </c>
       <c r="F12" s="3">
-        <v>0.5431444910556542</v>
+        <v>0.5431446161467421</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1329,7 +1330,7 @@
         <v>1.865292010949807</v>
       </c>
       <c r="F14" s="3">
-        <v>3.637363889319251</v>
+        <v>3.637364727037048</v>
       </c>
     </row>
   </sheetData>
@@ -1386,7 +1387,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809509277344</v>
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1406,7 +1407,7 @@
         <v>0.01798535747964639</v>
       </c>
       <c r="F3" s="3">
-        <v>0.01754828062675264</v>
+        <v>0.01754828630708088</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1426,7 +1427,7 @@
         <v>0.08267675643617589</v>
       </c>
       <c r="F4" s="3">
-        <v>0.0396860234248138</v>
+        <v>0.03968598396461956</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1446,7 +1447,7 @@
         <v>0.00683544605480675</v>
       </c>
       <c r="F5" s="3">
-        <v>0.00157498045527487</v>
+        <v>0.001574977323240041</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1466,7 +1467,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05249051910732176</v>
+        <v>-0.05248821566458358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1486,7 +1487,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470629158572999</v>
+        <v>1.470635920535974</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1494,19 +1495,19 @@
         <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>-0.05974788757676671</v>
+        <v>-0.05799800594496463</v>
       </c>
       <c r="C8" s="3">
-        <v>-0.04328047828198676</v>
+        <v>-0.04235724559895471</v>
       </c>
       <c r="D8" s="3">
-        <v>-0.04661371305828628</v>
+        <v>-0.04554397971420299</v>
       </c>
       <c r="E8" s="3">
-        <v>-0.1255507679335395</v>
+        <v>-0.1179890145847151</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.05478866077194264</v>
+        <v>-0.05331480146745704</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1514,19 +1515,19 @@
         <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>-0.06954379657081117</v>
+        <v>-0.06718072179566781</v>
       </c>
       <c r="C9" s="3">
-        <v>-0.05884111133361371</v>
+        <v>-0.05714343352132234</v>
       </c>
       <c r="D9" s="3">
-        <v>-0.06731872579096897</v>
+        <v>-0.06510282199709561</v>
       </c>
       <c r="E9" s="3">
-        <v>-0.1556441375478295</v>
+        <v>-0.1441362940579037</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.08013953248461748</v>
+        <v>-0.07701218969951162</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1534,19 +1535,19 @@
         <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>-0.07758490864213871</v>
+        <v>-0.07465154901957483</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.06564310427051488</v>
+        <v>-0.06353497497395366</v>
       </c>
       <c r="D10" s="3">
-        <v>-0.07713519228598358</v>
+        <v>-0.07423531109854076</v>
       </c>
       <c r="E10" s="3">
-        <v>-0.1684350095699264</v>
+        <v>-0.155013822350441</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.08986170774842375</v>
+        <v>-0.08594229392202379</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1554,19 +1555,19 @@
         <v>15</v>
       </c>
       <c r="B11" s="3">
-        <v>-0.08398727017367535</v>
+        <v>-0.08055703963017125</v>
       </c>
       <c r="C11" s="3">
-        <v>-0.08888368819397073</v>
+        <v>-0.08504801289619279</v>
       </c>
       <c r="D11" s="3">
-        <v>-0.09398170804669025</v>
+        <v>-0.08970058675715831</v>
       </c>
       <c r="E11" s="3">
-        <v>-0.1836567093057054</v>
+        <v>-0.1677785513268204</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.1215858604569134</v>
+        <v>-0.1144849050085754</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1586,7 +1587,7 @@
         <v>0.5210181173153532</v>
       </c>
       <c r="F12" s="3">
-        <v>0.5431444910556542</v>
+        <v>0.5431446161467421</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1626,7 +1627,7 @@
         <v>1.865292010949807</v>
       </c>
       <c r="F14" s="3">
-        <v>3.637363889319251</v>
+        <v>3.637364727037048</v>
       </c>
     </row>
   </sheetData>
@@ -1683,7 +1684,7 @@
         <v>43.63</v>
       </c>
       <c r="F2" s="2">
-        <v>191.3809509277344</v>
+        <v>191.3809661865234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1691,19 +1692,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>0.4125710786143765</v>
+        <v>0.03465597060360763</v>
       </c>
       <c r="C3" s="3">
-        <v>0.1051647568216076</v>
+        <v>0.008833839573015036</v>
       </c>
       <c r="D3" s="3">
-        <v>0.1162016562414957</v>
+        <v>0.009760939124285642</v>
       </c>
       <c r="E3" s="3">
-        <v>0.4496339369911597</v>
+        <v>0.03776925070725742</v>
       </c>
       <c r="F3" s="3">
-        <v>0.4387070156688158</v>
+        <v>0.03685140124486985</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1711,19 +1712,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="3">
-        <v>0.1913962061821985</v>
+        <v>0.05547189063155183</v>
       </c>
       <c r="C4" s="3">
-        <v>0.1384383400030983</v>
+        <v>0.04012324282203933</v>
       </c>
       <c r="D4" s="3">
-        <v>0.1537827237197764</v>
+        <v>0.04457046772956886</v>
       </c>
       <c r="E4" s="3">
-        <v>0.4133837821808794</v>
+        <v>0.1198100025669567</v>
       </c>
       <c r="F4" s="3">
-        <v>0.198430117124069</v>
+        <v>0.05751045451745348</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1731,19 +1732,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="3">
-        <v>0.03663250774093866</v>
+        <v>0.003077130650238848</v>
       </c>
       <c r="C5" s="3">
-        <v>0.01916517398281346</v>
+        <v>0.001609874614556331</v>
       </c>
       <c r="D5" s="3">
-        <v>0.02364912611467308</v>
+        <v>0.001986526593632539</v>
       </c>
       <c r="E5" s="3">
-        <v>0.1708861513701687</v>
+        <v>0.01435443671509417</v>
       </c>
       <c r="F5" s="3">
-        <v>0.03937451138187174</v>
+        <v>0.003307452378804086</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1763,7 +1764,7 @@
         <v>0.3558744450200944</v>
       </c>
       <c r="F6" s="3">
-        <v>-0.05249051910732176</v>
+        <v>-0.05248821566458358</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1783,7 +1784,7 @@
         <v>0.7185392133336488</v>
       </c>
       <c r="F7" s="3">
-        <v>1.470629158572999</v>
+        <v>1.470635920535974</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1791,19 +1792,19 @@
         <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>-0.2987394378838335</v>
+        <v>-0.08294049223427413</v>
       </c>
       <c r="C8" s="3">
-        <v>-0.2164023914099338</v>
+        <v>-0.0607929951813917</v>
       </c>
       <c r="D8" s="3">
-        <v>-0.2330685652914314</v>
+        <v>-0.06531872274428896</v>
       </c>
       <c r="E8" s="3">
-        <v>-0.6277538396676976</v>
+        <v>-0.1663489320221079</v>
       </c>
       <c r="F8" s="3">
-        <v>-0.2739433038597132</v>
+        <v>-0.07632621153963082</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1811,19 +1812,19 @@
         <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>-0.3477189828540558</v>
+        <v>-0.09586675600067596</v>
       </c>
       <c r="C9" s="3">
-        <v>-0.2942055566680685</v>
+        <v>-0.08173464394712393</v>
       </c>
       <c r="D9" s="3">
-        <v>-0.3365936289548448</v>
+        <v>-0.0929467329417244</v>
       </c>
       <c r="E9" s="3">
-        <v>-0.7782206877391473</v>
+        <v>-0.2019226716669809</v>
       </c>
       <c r="F9" s="3">
-        <v>-0.4006976624230874</v>
+        <v>-0.1096430311662466</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1831,19 +1832,19 @@
         <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>-0.3879245432106935</v>
+        <v>-0.1063411838753529</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.3282155213525744</v>
+        <v>-0.0907415442651075</v>
       </c>
       <c r="D10" s="3">
-        <v>-0.3856759614299178</v>
+        <v>-0.1057585957915729</v>
       </c>
       <c r="E10" s="3">
-        <v>-0.8421750478496322</v>
+        <v>-0.2165793652403061</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.4493085387421187</v>
+        <v>-0.1220993020676024</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1851,19 +1852,19 @@
         <v>15</v>
       </c>
       <c r="B11" s="3">
-        <v>-0.4199363508683768</v>
+        <v>-0.1145941197849433</v>
       </c>
       <c r="C11" s="3">
-        <v>-0.4444184409698536</v>
+        <v>-0.1208543551483093</v>
       </c>
       <c r="D11" s="3">
-        <v>-0.4699085402334512</v>
+        <v>-0.1273253158243038</v>
       </c>
       <c r="E11" s="3">
-        <v>-0.9182835465285266</v>
+        <v>-0.2336711219351461</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.6079293022845669</v>
+        <v>-0.1615451349056326</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1883,7 +1884,7 @@
         <v>0.5210181173153532</v>
       </c>
       <c r="F12" s="3">
-        <v>0.5431444910556542</v>
+        <v>0.5431446161467421</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1923,7 +1924,304 @@
         <v>1.865292010949807</v>
       </c>
       <c r="F14" s="3">
-        <v>3.637363889319251</v>
+        <v>3.637364727037048</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>161.74</v>
+      </c>
+      <c r="C2" s="2">
+        <v>190.829</v>
+      </c>
+      <c r="D2" s="2">
+        <v>683.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43.63</v>
+      </c>
+      <c r="F2" s="2">
+        <v>191.3809661865234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.4125710786143765</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.1051647568216076</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.1162016562414957</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.4496339369911597</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.438707157677022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.1913962061821985</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.1384383400030983</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1537827237197764</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.4133837821808794</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.1984299198230978</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.03663250774093866</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.01916517398281346</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.02364912611467308</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.1708861513701687</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.03937443308100102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.598275154235423</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-0.104956455941808</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-0.2001417301867452</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.3558744450200944</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-0.05248821566458358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.130009561889286</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.688795061363862</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.7875659701474236</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.7185392133336488</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.470635920535974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>-0.2582473431006131</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-0.1945888538675579</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-0.2079007388543198</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-0.4662105678841544</v>
+      </c>
+      <c r="F8" s="3">
+        <v>-0.2396248156230657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>-0.2937026700115168</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-0.2548766893648746</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-0.2858009892613433</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-0.5407776151820956</v>
+      </c>
+      <c r="F9" s="3">
+        <v>-0.3301465057954592</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>-0.3215364639872514</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-0.2797922171780177</v>
+      </c>
+      <c r="D10" s="3">
+        <v>-0.3200091667584076</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-0.5692274471813069</v>
+      </c>
+      <c r="F10" s="3">
+        <v>-0.3619303733051077</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3">
+        <v>-0.3429113583944799</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-0.358802938435328</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-0.3749405665416327</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-0.6007963321270422</v>
+      </c>
+      <c r="F11" s="3">
+        <v>-0.4555226173149048</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5257815340198895</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1165552785803567</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.104274499922256</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5210181173153532</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.5431446161467421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.1039095986491753</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-0.09780922394543157</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.1303597122302159</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.2793225480283115</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-0.1493236606462561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.059990038023909</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.191659374021654</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.799898205805385</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.865292010949807</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.637364727037048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>